<commit_message>
Dub phrases excel sheets
</commit_message>
<xml_diff>
--- a/Перевод.xlsx
+++ b/Перевод.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VityaSchel\Desktop\At Dead of Night ОЗВУЧКА\ru\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\At Dead of Night ОЗВУЧКА\ru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8C6576-3004-46E3-947C-E538B8D10867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09D20D4-ED4D-4399-9022-D5CBB84CB56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{43F2AE15-FF98-423E-8257-DE86D064BB25}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{43F2AE15-FF98-423E-8257-DE86D064BB25}"/>
   </bookViews>
   <sheets>
     <sheet name="Maya EVP Items (EVP-&gt;M_O.mp3)" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Intro video" sheetId="5" r:id="rId5"/>
     <sheet name="Amy" sheetId="6" r:id="rId6"/>
     <sheet name="Events EVP" sheetId="7" r:id="rId7"/>
+    <sheet name="Phrases" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="1229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="1302">
   <si>
     <t>M_O26B.mp3</t>
   </si>
@@ -3727,6 +3728,353 @@
   </si>
   <si>
     <t>Роуз</t>
+  </si>
+  <si>
+    <t>A2.mp3</t>
+  </si>
+  <si>
+    <t>A3.mp3</t>
+  </si>
+  <si>
+    <t>A4.mp3</t>
+  </si>
+  <si>
+    <t>A5.mp3</t>
+  </si>
+  <si>
+    <t>A6.mp3</t>
+  </si>
+  <si>
+    <t>P1.mp3</t>
+  </si>
+  <si>
+    <t>P3.mp3</t>
+  </si>
+  <si>
+    <t>P4.mp3</t>
+  </si>
+  <si>
+    <t>P5.mp3</t>
+  </si>
+  <si>
+    <t>P6.mp3</t>
+  </si>
+  <si>
+    <t>P7.mp3</t>
+  </si>
+  <si>
+    <t>P8.mp3</t>
+  </si>
+  <si>
+    <t>P9.mp3</t>
+  </si>
+  <si>
+    <t>H1.mp3</t>
+  </si>
+  <si>
+    <t>H2.mp3</t>
+  </si>
+  <si>
+    <t>H3.mp3</t>
+  </si>
+  <si>
+    <t>H4.mp3</t>
+  </si>
+  <si>
+    <t>H5.mp3</t>
+  </si>
+  <si>
+    <t>H6.mp3</t>
+  </si>
+  <si>
+    <t>H7.mp3</t>
+  </si>
+  <si>
+    <t>H8.mp3</t>
+  </si>
+  <si>
+    <t>H9.mp3</t>
+  </si>
+  <si>
+    <t>R1.mp3</t>
+  </si>
+  <si>
+    <t>R2.mp3</t>
+  </si>
+  <si>
+    <t>R3.mp3</t>
+  </si>
+  <si>
+    <t>R4.mp3</t>
+  </si>
+  <si>
+    <t>R5.mp3</t>
+  </si>
+  <si>
+    <t>R6.mp3</t>
+  </si>
+  <si>
+    <t>R7.mp3</t>
+  </si>
+  <si>
+    <t>R8.mp3</t>
+  </si>
+  <si>
+    <t>R9.mp3</t>
+  </si>
+  <si>
+    <t>V1.mp3</t>
+  </si>
+  <si>
+    <t>V2.mp3</t>
+  </si>
+  <si>
+    <t>V3.mp3</t>
+  </si>
+  <si>
+    <t>Epilogue.mp3</t>
+  </si>
+  <si>
+    <t>JimEndCorridor.mp3</t>
+  </si>
+  <si>
+    <t>JimEndAppear.mp3</t>
+  </si>
+  <si>
+    <t>JimEndTalk.mp3</t>
+  </si>
+  <si>
+    <t>Дамы и Господа,
+Поприветствуйте на сцене,
+ведущий вечернего шоу,
+Господин Хьюго Панч!
+АПЛОДИСМЕНТЫ
+Майя!
+Майя!
+Майя?
+Майя!
+ВСХЛИПЫВАНИЕ
+Прекрати, прекрати, прекрати, прекрати...
+Прекрати.
+Почему ты и дальше заставляешь меня делать это?
+Просто прекрати, прошу тебя.
+Просто прекрати, прекрати, пожалуйста...
+Ты всегда будешь делать это, Джимми.
+Я тут главный.
+Не ты.
+Я главный.</t>
+  </si>
+  <si>
+    <t>КРИКИ</t>
+  </si>
+  <si>
+    <t>КАШЕЛЬ</t>
+  </si>
+  <si>
+    <t>ХИХИКАНЬЕ</t>
+  </si>
+  <si>
+    <t>РАЗБИВАНИЕ ВЕЩЕЙ</t>
+  </si>
+  <si>
+    <t>Джимми, отдай! Это моё!
+Хватит красть мои вещи!</t>
+  </si>
+  <si>
+    <t>Я говорю тебе, Джимми, ты не можешь себя так вести!
+Ты ужасен...
+ГОЛОСА ИСЧЕЗАЮТ</t>
+  </si>
+  <si>
+    <t>СТУК В ДВЕРЬ
+Джимми?
+Я Доктор Боуз.
+Я пришел, чтобы немного поболтать, хорошо?
+Спасибо, Джимми, я ненадолго.</t>
+  </si>
+  <si>
+    <t>Это отличная идея, Джимми!
+Думаю, однажды ты станешь отличным поваром.
+Не мог бы ты принести ко мне в комнату, когда закончишь?
+Я буду ждать тебя, хорошо?</t>
+  </si>
+  <si>
+    <t>ПЛЕВКИ
+Джимми!</t>
+  </si>
+  <si>
+    <t>Это не навредит тебе Джимми.
+Все, что тебе нужно сделать, это остановиться и перестать двигаться!</t>
+  </si>
+  <si>
+    <t>Я бы никогда не применил такие меры к пациенту, Миссис Холл.
+Это противоречит всему, во что я верю.
+Вы должны понять, что он все выдумывает!</t>
+  </si>
+  <si>
+    <t>Ты не сможешь от меня так легко отвязаться, Джимми.
+Я думаю, нам следует начать сначала, а ты как думаешь?
+Почему на этот раз ты не сделаешь то, что я прошу?
+Это было бы хорошим началом, не так ли?</t>
+  </si>
+  <si>
+    <t>Это полиция, Мистер Боуз.
+Нам нужно, чтобы вы подошли к ресепшену.
+Вы можете открыть дверь, пожалуйста?</t>
+  </si>
+  <si>
+    <t>ЗВУКИ УДУШЬЯ
+ЗВУКИ СИГНАЛИЗАЦИИ ЛИФТА</t>
+  </si>
+  <si>
+    <t>Он это выдумал. Я говорю тебе, он лгал обо всем,
+Наверное, солгал и обо всём другом.
+Не неси чушь! Он бы не стал лгать о таком!
+Ты уверена в этом?
+Он лжет обо всем! Открой свои чёртовы глаза, Роуз!
+Да, верно! Теперь уходи!
+Я не слушаю Харви, ты на него просто наговариваешь.
+Это правда!</t>
+  </si>
+  <si>
+    <t>СТУК В ДВЕРЬ
+Джимми?
+Я знаю ты слышишь меня!
+Я знаю, что ты выдумал свою маленькую историю про психиатра.
+Я знаю, откуда ты это взял!
+Я знал, что читал об этом раньше, в твоих чертовых вырезках из газет!
+Выходи сюда!
+Джимми!</t>
+  </si>
+  <si>
+    <t>ИСКРЫ ЭЛЕКТРОПРОВОДКИ
+КРИЧИТ ОТ БОЛИ
+Джимми!</t>
+  </si>
+  <si>
+    <t>КРИКИ ОТ БОЛИ
+Джимми!</t>
+  </si>
+  <si>
+    <t>Ты можешь остаться здесь на ночь, Джимми!
+С меня достаточно.
+СТУКИ В ДВЕРЬ</t>
+  </si>
+  <si>
+    <t>ПОЖАРНАЯ ТРЕВОГА
+Джимми, не будь дураком, открой дверь!
+Ты же погибнешь, идиот! Открой дверь!</t>
+  </si>
+  <si>
+    <t>Убирайся из отеля Джимми.
+Убирайся из моего отеля ...
+Это мой отель. Убирайся из моего отеля, Джимми.</t>
+  </si>
+  <si>
+    <t>Убирайся из моего отеля.
+Это МОЙ отель.</t>
+  </si>
+  <si>
+    <t>Харви собирался застрелить Джимми.
+Это была просто открывалка для писем. Это была самооборона! Смотрите!</t>
+  </si>
+  <si>
+    <t>Леди и джентльмены.
+Поприветствуйте на сцене,
+ведущий вечернего шоу,
+Господин Хьюго Панч!
+МУЗЫКА И АПЛОДИСМЕНТЫ</t>
+  </si>
+  <si>
+    <t>Это просто его комедия.
+Это его чувство юмора!
+Извините, если это вас задело...
+Прошу прощения...</t>
+  </si>
+  <si>
+    <t>СТУК В ДВЕРЬ
+Миссис Холл?
+Миссис Холл, можно вас на пару слов?</t>
+  </si>
+  <si>
+    <t>Джимми?
+КРИКИ
+Джимми! Что ты наделал! Джимми!</t>
+  </si>
+  <si>
+    <t>ДЕТСКИЙ ПЛАЧ
+Ты будешь делать то, что я тебе сказал! Ты понял?
+Глупый негодник!
+УДАРЫ ПО РЕБЕНКУ
+УДАР БИТОЙ ПО МУЖЧИНЕ</t>
+  </si>
+  <si>
+    <t>Вот!
+ГОНГ
+Я Великий Хьюго!
+Я самый особенный.
+Я свет, озаряющий тьму.
+Я единственный хозяин.</t>
+  </si>
+  <si>
+    <t>ЖЕНСКИЙ ПЛАЧ
+Не покупай ничего без моего разрешения!
+ЗВУК БЬЮЩЕГОСЯ СТЕКЛА
+Я не позволю тебе разрушить мою жизнь!
+ЕЩЁ ЗВУК БЬЮЩЕГОСЯ СТЕКЛА
+Твоя жизнь ничего не значит!
+Ты понимаешь, о чем я тебе говорю?
+ЗВУК УДАРОВ И ЖЕНСКИЕ КРИКИ</t>
+  </si>
+  <si>
+    <t>ДЕТСКИЙ ПЛАЧ
+Сиди спокойно!
+ЗВУК УДАРОВ
+Ты глупый, мелкий бесстыдник!
+Делай что говорят!
+ЖЕНСКИЕ КРИКИ&lt;br&gt;Нет!</t>
+  </si>
+  <si>
+    <t>Добро пожаловать в могилу Хьюго!
+Мамин маленький секрет.
+Знаешь ли, она сама смешала бетон,
+затем вылила всё на его безжизненное тело
+и смотрела, как бетон засыхает.
+Она думала, что так избавится от Хьюго.
+Но она не понимала, Майя.
+Видишь ли, Хьюго был просто одним из нас.
+Просто очередным бревном в огне.
+Он выгорел.
+Но огонь веками горит в этих коридорах.
+Очищая путь...
+Освещая тьму...
+Опустошая старых, бедных, слабых.
+И этот огонь есть в тебе тоже, Майя.
+Я вижу!
+Судьбой предписано, что мы должны быть вместе. Ты и я.
+Ты именно та, кого я ждал.
+И поэтому я не могу дать тебе уйти.
+Ты останешься здесь со мной, Майя.
+Навечно.</t>
+  </si>
+  <si>
+    <t>Разговариваешь с мёртвыми, Майя?
+Я знаю, что Хьюго твой отец, Джимми.
+Я нашла твоё свидетельство о рождении, и я знаю, что Роуз пыталась убить его.
+Попытка вышла неудачной, не так ли.
+Тогда где же он сейчас?
+СМЕХ
+Так почему бы тебе не пойти и не встретиться с ним?
+Пора представить тебя семье, Майя.
+СМЕХ</t>
+  </si>
+  <si>
+    <t>Привет Майя!
+Майя!
+Майя!
+СИЛЬНЫЙ СТУК В ДВЕРЬ
+Тебе не сбежать от меня, Майя!
+Открой дверь!</t>
   </si>
 </sst>
 </file>
@@ -3916,46 +4264,11 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFAFAF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3970,13 +4283,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF99FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4309,10 +4615,477 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF985361-8433-4565-99F1-1AC2059D9C02}">
+  <sheetPr codeName="Лист1"/>
   <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAE930C-277F-4EA1-82A0-964A829E84DD}">
+  <sheetPr codeName="Лист2"/>
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4331,471 +5104,6 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>0</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>1</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>2</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAE930C-277F-4EA1-82A0-964A829E84DD}">
-  <dimension ref="A1:B28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
         <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -5017,10 +5325,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD0B0A8-85A8-47EF-A491-A4292D08A4BF}">
+  <sheetPr codeName="Лист3"/>
   <dimension ref="A1:D158"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B150" sqref="B150"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A37" sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6313,6 +6622,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E7FB80-922A-496D-94A6-6B5F1159886E}">
+  <sheetPr codeName="Лист4"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
@@ -6380,6 +6690,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A4CDD3-149D-4880-9F8B-8BC6A1903D82}">
+  <sheetPr codeName="Лист5"/>
   <dimension ref="A1:G96"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
@@ -7764,6 +8075,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8982577E-577F-479C-AE30-9EF52371E4AE}">
+  <sheetPr codeName="Лист6"/>
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView topLeftCell="C28" zoomScaleNormal="100" workbookViewId="0">
@@ -7896,7 +8208,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>827</v>
       </c>
@@ -7912,7 +8224,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>829</v>
       </c>
@@ -7920,7 +8232,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>826</v>
       </c>
@@ -8024,7 +8336,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>856</v>
       </c>
@@ -8071,10 +8383,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A097F482-9E4B-4DA0-95EF-7D7F45549731}">
+  <sheetPr codeName="Лист7"/>
   <dimension ref="A1:D195"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10227,19 +10540,347 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Харви"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Роуз"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Боуз"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Эмми"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDF31A8-3CD1-4E1D-B9C6-E09ABA938F23}">
+  <dimension ref="A1:B39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>